<commit_message>
Updated input forms with dummy template values
</commit_message>
<xml_diff>
--- a/git_discovery_input_form.xlsx
+++ b/git_discovery_input_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romy\Desktop\DevOpsServer2020TOADO_Migration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsure\OneDrive\Documents\1_Official\DMAP\New_Development\DevOpsServer2020TOADO_Migration\multiple_project_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E667EE59-0527-44A0-B762-A8CA62757C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED92DC7-18B5-444A-9543-92D898A30357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Server URL</t>
   </si>
@@ -53,19 +53,25 @@
     <t>Branch Name</t>
   </si>
   <si>
-    <t>http://172.191.4.85/TestCollection</t>
-  </si>
-  <si>
-    <t>uhepmbf5obmvbwfmxajdzju25rfmabbmovw5judh7f25pqyudpia</t>
-  </si>
-  <si>
-    <t>opserver</t>
-  </si>
-  <si>
-    <t>qaserver</t>
-  </si>
-  <si>
-    <t>dspot</t>
+    <t>project1</t>
+  </si>
+  <si>
+    <t>http://128.0.0.1/TestCollection</t>
+  </si>
+  <si>
+    <t>project2</t>
+  </si>
+  <si>
+    <t>repo1</t>
+  </si>
+  <si>
+    <t>adad87adad8ds4449m434344mmnbnbb43434</t>
+  </si>
+  <si>
+    <t>repo2</t>
+  </si>
+  <si>
+    <t>project3</t>
   </si>
 </sst>
 </file>
@@ -343,11 +349,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -377,36 +381,47 @@
     </row>
     <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{643D8D03-F719-4D55-9590-924B212FB597}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{B5F649D1-7BD7-43C9-BE03-7A66E77436C5}"/>
+    <hyperlink ref="A3:A4" r:id="rId2" display="http://128.0.0.1/TestCollection" xr:uid="{FA0E0052-90DB-4024-B34B-8B02F2177F2B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>